<commit_message>
add h_p h_q h_r h_s
</commit_message>
<xml_diff>
--- a/hydrogen_comps/H10_chain/H10_0.60/H10_0.60_energies.xlsx
+++ b/hydrogen_comps/H10_chain/H10_0.60/H10_0.60_energies.xlsx
@@ -447,7 +447,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>-0.1043788321</v>
+        <v>-0.1043788461</v>
       </c>
     </row>
     <row r="3">
@@ -467,7 +467,7 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>-4.7862948</v>
+        <v>-4.78629482</v>
       </c>
     </row>
   </sheetData>

</xml_diff>